<commit_message>
Bug nei check ricerce locali risolto
</commit_message>
<xml_diff>
--- a/PS-VRP/Dati_output/Problemi_lettura_Excel.xlsx
+++ b/PS-VRP/Dati_output/Problemi_lettura_Excel.xlsx
@@ -423,7 +423,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P10"/>
+  <dimension ref="A1:P8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -536,7 +536,7 @@
         <v>233333</v>
       </c>
       <c r="B2" s="1" t="n">
-        <v>45845</v>
+        <v>45903</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -599,10 +599,10 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>251310</v>
+        <v>251702</v>
       </c>
       <c r="B3" s="1" t="n">
-        <v>45770</v>
+        <v>45903</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -610,20 +610,20 @@
         </is>
       </c>
       <c r="D3" s="1" t="n">
-        <v>45769</v>
+        <v>45853</v>
       </c>
       <c r="E3" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>8611</v>
+        <v>60063</v>
       </c>
       <c r="G3" t="n">
-        <v>336</v>
+        <v>4607</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>1</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
@@ -632,10 +632,10 @@
         </is>
       </c>
       <c r="J3" t="n">
-        <v>410</v>
+        <v>340</v>
       </c>
       <c r="K3" t="n">
-        <v>820</v>
+        <v>1020</v>
       </c>
       <c r="L3" s="2" t="inlineStr">
         <is>
@@ -663,56 +663,56 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>251905</v>
-      </c>
-      <c r="B4" s="2" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
+        <v>251310</v>
+      </c>
+      <c r="B4" s="1" t="n">
+        <v>45770</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>IN STAMPA</t>
+          <t>STAMPATO</t>
         </is>
       </c>
       <c r="D4" s="1" t="n">
-        <v>45805</v>
+        <v>45769</v>
       </c>
       <c r="E4" t="n">
+        <v>6</v>
+      </c>
+      <c r="F4" t="n">
+        <v>8611</v>
+      </c>
+      <c r="G4" t="n">
+        <v>336</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>bobina</t>
+        </is>
+      </c>
+      <c r="J4" t="n">
+        <v>410</v>
+      </c>
+      <c r="K4" t="n">
+        <v>820</v>
+      </c>
+      <c r="L4" s="2" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>Dati OK</t>
+        </is>
+      </c>
+      <c r="N4" t="n">
         <v>1</v>
-      </c>
-      <c r="F4" t="n">
-        <v>13841</v>
-      </c>
-      <c r="G4" t="n">
-        <v>1000</v>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>bobina</t>
-        </is>
-      </c>
-      <c r="J4" t="n">
-        <v>165</v>
-      </c>
-      <c r="K4" t="n">
-        <v>825</v>
-      </c>
-      <c r="L4" t="n">
-        <v>76</v>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>Dati OK</t>
-        </is>
-      </c>
-      <c r="N4" t="n">
-        <v>0</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
@@ -727,33 +727,31 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>252666</v>
-      </c>
-      <c r="B5" s="2" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
+        <v>252683</v>
+      </c>
+      <c r="B5" s="1" t="n">
+        <v>45903</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>DA STAMPARE</t>
+          <t>STAMPATO</t>
         </is>
       </c>
       <c r="D5" s="1" t="n">
         <v>45901</v>
       </c>
       <c r="E5" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F5" t="n">
-        <v>13175</v>
+        <v>19381</v>
       </c>
       <c r="G5" t="n">
-        <v>600</v>
+        <v>2000</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>CAMPO VUOTO</t>
+          <t>5</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
@@ -762,13 +760,15 @@
         </is>
       </c>
       <c r="J5" t="n">
-        <v>680</v>
+        <v>820</v>
       </c>
       <c r="K5" t="n">
-        <v>680</v>
-      </c>
-      <c r="L5" t="n">
-        <v>70</v>
+        <v>820</v>
+      </c>
+      <c r="L5" s="2" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
@@ -776,87 +776,87 @@
         </is>
       </c>
       <c r="N5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-      <c r="P5" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="P5" t="n">
+        <v>40295</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>251704</v>
+        <v>252459</v>
       </c>
       <c r="B6" s="1" t="n">
-        <v>45846</v>
+        <v>45855</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
           <t>STAMPATO</t>
         </is>
       </c>
-      <c r="D6" s="1" t="n">
-        <v>45848</v>
+      <c r="D6" s="2" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
       </c>
       <c r="E6" t="n">
+        <v>1</v>
+      </c>
+      <c r="F6" t="n">
+        <v>4000</v>
+      </c>
+      <c r="G6" t="n">
+        <v>91</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>foglio</t>
+        </is>
+      </c>
+      <c r="J6" t="n">
+        <v>200</v>
+      </c>
+      <c r="K6" t="n">
+        <v>480</v>
+      </c>
+      <c r="L6" t="n">
         <v>0</v>
       </c>
-      <c r="F6" t="n">
-        <v>28904</v>
-      </c>
-      <c r="G6" t="n">
-        <v>2217</v>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>bobina</t>
-        </is>
-      </c>
-      <c r="J6" t="n">
-        <v>340</v>
-      </c>
-      <c r="K6" t="n">
-        <v>1020</v>
-      </c>
-      <c r="L6" s="2" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
       <c r="M6" t="inlineStr">
         <is>
           <t>Dati OK</t>
         </is>
       </c>
       <c r="N6" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="P6" t="n">
-        <v>40054</v>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>252453</v>
+        <v>252596</v>
       </c>
       <c r="B7" s="1" t="n">
-        <v>45845</v>
+        <v>45904</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -864,32 +864,32 @@
         </is>
       </c>
       <c r="D7" s="1" t="n">
-        <v>45835</v>
+        <v>45873</v>
       </c>
       <c r="E7" t="n">
         <v>1</v>
       </c>
       <c r="F7" t="n">
-        <v>2990</v>
+        <v>3497</v>
       </c>
       <c r="G7" t="n">
-        <v>169</v>
+        <v>305</v>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>3 / 4</t>
-        </is>
-      </c>
-      <c r="I7" s="2" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
+          <t>5 / 9</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>bobina</t>
         </is>
       </c>
       <c r="J7" t="n">
-        <v>190</v>
+        <v>470</v>
       </c>
       <c r="K7" t="n">
-        <v>760</v>
+        <v>940</v>
       </c>
       <c r="L7" s="2" t="inlineStr">
         <is>
@@ -898,7 +898,7 @@
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ERR tipologia incarto non definita</t>
+          <t>Dati OK</t>
         </is>
       </c>
       <c r="N7" t="n">
@@ -906,21 +906,19 @@
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-      <c r="P7" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="P7" t="n">
+        <v>40295</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>252983</v>
+        <v>251624</v>
       </c>
       <c r="B8" s="1" t="n">
-        <v>45847</v>
+        <v>45908</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -928,181 +926,53 @@
         </is>
       </c>
       <c r="D8" s="1" t="n">
-        <v>45862</v>
+        <v>45895</v>
       </c>
       <c r="E8" t="n">
+        <v>1</v>
+      </c>
+      <c r="F8" t="n">
+        <v>10957</v>
+      </c>
+      <c r="G8" t="n">
+        <v>574</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>bobina</t>
+        </is>
+      </c>
+      <c r="J8" t="n">
+        <v>155</v>
+      </c>
+      <c r="K8" t="n">
+        <v>620</v>
+      </c>
+      <c r="L8" s="2" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>Dati OK</t>
+        </is>
+      </c>
+      <c r="N8" t="n">
         <v>0</v>
       </c>
-      <c r="F8" t="n">
-        <v>1912</v>
-      </c>
-      <c r="G8" t="n">
-        <v>97</v>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>bobina</t>
-        </is>
-      </c>
-      <c r="J8" t="n">
-        <v>85</v>
-      </c>
-      <c r="K8" t="n">
-        <v>425</v>
-      </c>
-      <c r="L8" s="2" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t>Dati OK</t>
-        </is>
-      </c>
-      <c r="N8" t="n">
-        <v>4</v>
-      </c>
       <c r="O8" t="inlineStr">
         <is>
           <t>X</t>
         </is>
       </c>
       <c r="P8" t="n">
-        <v>40055</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>252450</v>
-      </c>
-      <c r="B9" s="1" t="n">
-        <v>45852</v>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>IN STAMPA</t>
-        </is>
-      </c>
-      <c r="D9" s="1" t="n">
-        <v>45849</v>
-      </c>
-      <c r="E9" t="n">
-        <v>1</v>
-      </c>
-      <c r="F9" t="n">
-        <v>5718</v>
-      </c>
-      <c r="G9" t="n">
-        <v>300</v>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>bobina</t>
-        </is>
-      </c>
-      <c r="J9" t="n">
-        <v>390</v>
-      </c>
-      <c r="K9" t="n">
-        <v>780</v>
-      </c>
-      <c r="L9" s="2" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-      <c r="M9" t="inlineStr">
-        <is>
-          <t>Dati OK</t>
-        </is>
-      </c>
-      <c r="N9" t="n">
-        <v>0</v>
-      </c>
-      <c r="O9" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-      <c r="P9" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>252354</v>
-      </c>
-      <c r="B10" s="1" t="n">
-        <v>45849</v>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>IN STAMPA</t>
-        </is>
-      </c>
-      <c r="D10" s="1" t="n">
-        <v>45847</v>
-      </c>
-      <c r="E10" t="n">
-        <v>6</v>
-      </c>
-      <c r="F10" t="n">
-        <v>5060</v>
-      </c>
-      <c r="G10" t="n">
-        <v>100</v>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>bobina</t>
-        </is>
-      </c>
-      <c r="J10" t="n">
-        <v>85</v>
-      </c>
-      <c r="K10" t="n">
-        <v>595</v>
-      </c>
-      <c r="L10" s="2" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t>Dati OK</t>
-        </is>
-      </c>
-      <c r="N10" t="n">
-        <v>2</v>
-      </c>
-      <c r="O10" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-      <c r="P10" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
+        <v>40308</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Risoluzione bug check nelle ricerche locali
</commit_message>
<xml_diff>
--- a/PS-VRP/Dati_output/Problemi_lettura_Excel.xlsx
+++ b/PS-VRP/Dati_output/Problemi_lettura_Excel.xlsx
@@ -423,7 +423,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P10"/>
+  <dimension ref="A1:P8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -536,7 +536,7 @@
         <v>233333</v>
       </c>
       <c r="B2" s="1" t="n">
-        <v>45845</v>
+        <v>45903</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -599,10 +599,10 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>251310</v>
+        <v>251702</v>
       </c>
       <c r="B3" s="1" t="n">
-        <v>45770</v>
+        <v>45903</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -610,20 +610,20 @@
         </is>
       </c>
       <c r="D3" s="1" t="n">
-        <v>45769</v>
+        <v>45853</v>
       </c>
       <c r="E3" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>8611</v>
+        <v>60063</v>
       </c>
       <c r="G3" t="n">
-        <v>336</v>
+        <v>4607</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>1</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
@@ -632,10 +632,10 @@
         </is>
       </c>
       <c r="J3" t="n">
-        <v>410</v>
+        <v>340</v>
       </c>
       <c r="K3" t="n">
-        <v>820</v>
+        <v>1020</v>
       </c>
       <c r="L3" s="2" t="inlineStr">
         <is>
@@ -663,56 +663,56 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>251905</v>
-      </c>
-      <c r="B4" s="2" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
+        <v>251310</v>
+      </c>
+      <c r="B4" s="1" t="n">
+        <v>45770</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>IN STAMPA</t>
+          <t>STAMPATO</t>
         </is>
       </c>
       <c r="D4" s="1" t="n">
-        <v>45805</v>
+        <v>45769</v>
       </c>
       <c r="E4" t="n">
+        <v>6</v>
+      </c>
+      <c r="F4" t="n">
+        <v>8611</v>
+      </c>
+      <c r="G4" t="n">
+        <v>336</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>bobina</t>
+        </is>
+      </c>
+      <c r="J4" t="n">
+        <v>410</v>
+      </c>
+      <c r="K4" t="n">
+        <v>820</v>
+      </c>
+      <c r="L4" s="2" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>Dati OK</t>
+        </is>
+      </c>
+      <c r="N4" t="n">
         <v>1</v>
-      </c>
-      <c r="F4" t="n">
-        <v>13841</v>
-      </c>
-      <c r="G4" t="n">
-        <v>1000</v>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>bobina</t>
-        </is>
-      </c>
-      <c r="J4" t="n">
-        <v>165</v>
-      </c>
-      <c r="K4" t="n">
-        <v>825</v>
-      </c>
-      <c r="L4" t="n">
-        <v>76</v>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>Dati OK</t>
-        </is>
-      </c>
-      <c r="N4" t="n">
-        <v>0</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
@@ -727,33 +727,31 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>252666</v>
-      </c>
-      <c r="B5" s="2" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
+        <v>252683</v>
+      </c>
+      <c r="B5" s="1" t="n">
+        <v>45903</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>DA STAMPARE</t>
+          <t>STAMPATO</t>
         </is>
       </c>
       <c r="D5" s="1" t="n">
         <v>45901</v>
       </c>
       <c r="E5" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F5" t="n">
-        <v>13175</v>
+        <v>19381</v>
       </c>
       <c r="G5" t="n">
-        <v>600</v>
+        <v>2000</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>CAMPO VUOTO</t>
+          <t>5</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
@@ -762,13 +760,15 @@
         </is>
       </c>
       <c r="J5" t="n">
-        <v>680</v>
+        <v>820</v>
       </c>
       <c r="K5" t="n">
-        <v>680</v>
-      </c>
-      <c r="L5" t="n">
-        <v>70</v>
+        <v>820</v>
+      </c>
+      <c r="L5" s="2" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
@@ -776,87 +776,87 @@
         </is>
       </c>
       <c r="N5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-      <c r="P5" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="P5" t="n">
+        <v>40295</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>251704</v>
+        <v>252459</v>
       </c>
       <c r="B6" s="1" t="n">
-        <v>45846</v>
+        <v>45855</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
           <t>STAMPATO</t>
         </is>
       </c>
-      <c r="D6" s="1" t="n">
-        <v>45848</v>
+      <c r="D6" s="2" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
       </c>
       <c r="E6" t="n">
+        <v>1</v>
+      </c>
+      <c r="F6" t="n">
+        <v>4000</v>
+      </c>
+      <c r="G6" t="n">
+        <v>91</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>foglio</t>
+        </is>
+      </c>
+      <c r="J6" t="n">
+        <v>200</v>
+      </c>
+      <c r="K6" t="n">
+        <v>480</v>
+      </c>
+      <c r="L6" t="n">
         <v>0</v>
       </c>
-      <c r="F6" t="n">
-        <v>28904</v>
-      </c>
-      <c r="G6" t="n">
-        <v>2217</v>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>bobina</t>
-        </is>
-      </c>
-      <c r="J6" t="n">
-        <v>340</v>
-      </c>
-      <c r="K6" t="n">
-        <v>1020</v>
-      </c>
-      <c r="L6" s="2" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
       <c r="M6" t="inlineStr">
         <is>
           <t>Dati OK</t>
         </is>
       </c>
       <c r="N6" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="P6" t="n">
-        <v>40054</v>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>252453</v>
+        <v>252596</v>
       </c>
       <c r="B7" s="1" t="n">
-        <v>45845</v>
+        <v>45904</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -864,32 +864,32 @@
         </is>
       </c>
       <c r="D7" s="1" t="n">
-        <v>45835</v>
+        <v>45873</v>
       </c>
       <c r="E7" t="n">
         <v>1</v>
       </c>
       <c r="F7" t="n">
-        <v>2990</v>
+        <v>3497</v>
       </c>
       <c r="G7" t="n">
-        <v>169</v>
+        <v>305</v>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>3 / 4</t>
-        </is>
-      </c>
-      <c r="I7" s="2" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
+          <t>5 / 9</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>bobina</t>
         </is>
       </c>
       <c r="J7" t="n">
-        <v>190</v>
+        <v>470</v>
       </c>
       <c r="K7" t="n">
-        <v>760</v>
+        <v>940</v>
       </c>
       <c r="L7" s="2" t="inlineStr">
         <is>
@@ -898,7 +898,7 @@
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ERR tipologia incarto non definita</t>
+          <t>Dati OK</t>
         </is>
       </c>
       <c r="N7" t="n">
@@ -906,21 +906,19 @@
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-      <c r="P7" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="P7" t="n">
+        <v>40295</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>252983</v>
+        <v>251624</v>
       </c>
       <c r="B8" s="1" t="n">
-        <v>45847</v>
+        <v>45908</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -928,181 +926,53 @@
         </is>
       </c>
       <c r="D8" s="1" t="n">
-        <v>45862</v>
+        <v>45895</v>
       </c>
       <c r="E8" t="n">
+        <v>1</v>
+      </c>
+      <c r="F8" t="n">
+        <v>10957</v>
+      </c>
+      <c r="G8" t="n">
+        <v>574</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>bobina</t>
+        </is>
+      </c>
+      <c r="J8" t="n">
+        <v>155</v>
+      </c>
+      <c r="K8" t="n">
+        <v>620</v>
+      </c>
+      <c r="L8" s="2" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>Dati OK</t>
+        </is>
+      </c>
+      <c r="N8" t="n">
         <v>0</v>
       </c>
-      <c r="F8" t="n">
-        <v>1912</v>
-      </c>
-      <c r="G8" t="n">
-        <v>97</v>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>bobina</t>
-        </is>
-      </c>
-      <c r="J8" t="n">
-        <v>85</v>
-      </c>
-      <c r="K8" t="n">
-        <v>425</v>
-      </c>
-      <c r="L8" s="2" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t>Dati OK</t>
-        </is>
-      </c>
-      <c r="N8" t="n">
-        <v>4</v>
-      </c>
       <c r="O8" t="inlineStr">
         <is>
           <t>X</t>
         </is>
       </c>
       <c r="P8" t="n">
-        <v>40055</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>252450</v>
-      </c>
-      <c r="B9" s="1" t="n">
-        <v>45852</v>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>IN STAMPA</t>
-        </is>
-      </c>
-      <c r="D9" s="1" t="n">
-        <v>45849</v>
-      </c>
-      <c r="E9" t="n">
-        <v>1</v>
-      </c>
-      <c r="F9" t="n">
-        <v>5718</v>
-      </c>
-      <c r="G9" t="n">
-        <v>300</v>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>bobina</t>
-        </is>
-      </c>
-      <c r="J9" t="n">
-        <v>390</v>
-      </c>
-      <c r="K9" t="n">
-        <v>780</v>
-      </c>
-      <c r="L9" s="2" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-      <c r="M9" t="inlineStr">
-        <is>
-          <t>Dati OK</t>
-        </is>
-      </c>
-      <c r="N9" t="n">
-        <v>0</v>
-      </c>
-      <c r="O9" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-      <c r="P9" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>252354</v>
-      </c>
-      <c r="B10" s="1" t="n">
-        <v>45849</v>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>IN STAMPA</t>
-        </is>
-      </c>
-      <c r="D10" s="1" t="n">
-        <v>45847</v>
-      </c>
-      <c r="E10" t="n">
-        <v>6</v>
-      </c>
-      <c r="F10" t="n">
-        <v>5060</v>
-      </c>
-      <c r="G10" t="n">
-        <v>100</v>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>bobina</t>
-        </is>
-      </c>
-      <c r="J10" t="n">
-        <v>85</v>
-      </c>
-      <c r="K10" t="n">
-        <v>595</v>
-      </c>
-      <c r="L10" s="2" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t>Dati OK</t>
-        </is>
-      </c>
-      <c r="N10" t="n">
-        <v>2</v>
-      </c>
-      <c r="O10" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-      <c r="P10" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
+        <v>40308</v>
       </c>
     </row>
   </sheetData>

</xml_diff>